<commit_message>
chore: include Date for Week 7 records; refresh cleaned file
</commit_message>
<xml_diff>
--- a/American_Healthcare_Class_Cleaned.xlsx
+++ b/American_Healthcare_Class_Cleaned.xlsx
@@ -656,7 +656,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -862,7 +866,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -1068,7 +1076,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -1274,7 +1286,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -1480,7 +1496,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -1686,7 +1706,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -1892,7 +1916,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -2098,7 +2126,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D57" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -2304,7 +2336,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -2510,7 +2546,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D71" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -2716,7 +2756,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D78" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -2922,7 +2966,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D85" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -3128,7 +3176,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D92" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -3334,7 +3386,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr"/>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D99" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -3540,7 +3596,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr"/>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D106" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -3746,7 +3806,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr"/>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D113" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -3952,7 +4016,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D120" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -4158,7 +4226,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr"/>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D127" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -4364,7 +4436,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr"/>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D134" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
@@ -4570,7 +4646,11 @@
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr"/>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
       <c r="D141" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>

</xml_diff>

<commit_message>
data: append Week 8 to cleaned file; improve week detection and include Date; refresh dashboards and scripts
</commit_message>
<xml_diff>
--- a/American_Healthcare_Class_Cleaned.xlsx
+++ b/American_Healthcare_Class_Cleaned.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -678,22 +678,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Alisha Ealias</t>
+          <t>Akshay Venkatesh</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -713,21 +713,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -743,21 +743,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -773,21 +773,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -803,21 +803,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -833,21 +833,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -863,21 +863,21 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -888,60 +888,60 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Anika Rahman Maria</t>
+          <t>Alisha Ealias</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Anika Rahman Maria</t>
+          <t>Alisha Ealias</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
@@ -953,17 +953,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -983,17 +983,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
@@ -1013,25 +1013,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
@@ -1043,17 +1043,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1073,17 +1073,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1098,26 +1098,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Astha Gungun Patel</t>
+          <t>Anika Rahman Maria</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1128,26 +1128,26 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Astha Gungun Patel</t>
+          <t>Anika Rahman Maria</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1158,30 +1158,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Astha Gungun Patel</t>
+          <t>Anika Rahman Maria</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
@@ -1193,17 +1193,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1223,21 +1223,21 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1253,25 +1253,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
@@ -1283,21 +1283,21 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1308,26 +1308,26 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Bhavishya Teki</t>
+          <t>Astha Gungun Patel</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1338,26 +1338,26 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Bhavishya Teki</t>
+          <t>Astha Gungun Patel</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1368,26 +1368,26 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bhavishya Teki</t>
+          <t>Astha Gungun Patel</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1398,22 +1398,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bhavishya Teki</t>
+          <t>Astha Gungun Patel</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1433,21 +1433,21 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1463,17 +1463,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1493,17 +1493,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1518,22 +1518,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bilegt Batkhorol</t>
+          <t>Bhavishya Teki</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1548,22 +1548,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Bilegt Batkhorol</t>
+          <t>Bhavishya Teki</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1578,22 +1578,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bilegt Batkhorol</t>
+          <t>Bhavishya Teki</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1608,26 +1608,26 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Bilegt Batkhorol</t>
+          <t>Bhavishya Teki</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1638,22 +1638,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bilegt Batkhorol</t>
+          <t>Bhavishya Teki</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
@@ -1673,21 +1673,21 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1703,21 +1703,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1728,26 +1728,26 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Deepika Joyce Chintha</t>
+          <t>Bilegt Batkhorol</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1758,22 +1758,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Deepika Joyce Chintha</t>
+          <t>Bilegt Batkhorol</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1781,29 +1781,29 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Deepika Joyce Chintha</t>
+          <t>Bilegt Batkhorol</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1818,22 +1818,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Deepika Joyce Chintha</t>
+          <t>Bilegt Batkhorol</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1848,22 +1848,22 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Deepika Joyce Chintha</t>
+          <t>Bilegt Batkhorol</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1878,22 +1878,22 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Deepika Joyce Chintha</t>
+          <t>Bilegt Batkhorol</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1913,21 +1913,21 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1938,52 +1938,52 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1991,33 +1991,33 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2028,26 +2028,26 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2058,26 +2058,26 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2088,26 +2088,26 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2118,26 +2118,26 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Julia Key</t>
+          <t>Deepika Joyce Chintha</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2148,7 +2148,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2201,14 +2201,14 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2227,7 +2227,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2238,7 +2238,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2268,7 +2268,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2287,7 +2287,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2298,7 +2298,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2328,7 +2328,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Kai Ern Caius Lee</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2347,7 +2347,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -2358,26 +2358,26 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Julia Key</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -2388,26 +2388,26 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -2418,26 +2418,26 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -2448,22 +2448,22 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2478,26 +2478,26 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2508,26 +2508,26 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -2538,26 +2538,26 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Kirti Gautam</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -2568,26 +2568,26 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -2598,26 +2598,26 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kai Ern Caius Lee</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -2628,26 +2628,26 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -2658,22 +2658,22 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2688,26 +2688,26 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -2718,26 +2718,26 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -2748,26 +2748,26 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Mary O'Reilly</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -2778,22 +2778,22 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2808,22 +2808,22 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2838,26 +2838,26 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Kirti Gautam</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -2868,26 +2868,26 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -2898,56 +2898,56 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -2958,26 +2958,26 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Michael Madden</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -2988,26 +2988,26 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -3018,26 +3018,26 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -3048,26 +3048,26 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -3078,26 +3078,26 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Mary O'Reilly</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -3108,26 +3108,26 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -3138,26 +3138,26 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -3168,26 +3168,26 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Prakruthi Jayant</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -3198,26 +3198,26 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -3228,56 +3228,56 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -3288,26 +3288,26 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -3318,26 +3318,26 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Michael Madden</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
@@ -3348,22 +3348,22 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -3378,26 +3378,26 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Priyanka Umesh Patil</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -3408,86 +3408,86 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -3498,26 +3498,26 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -3528,56 +3528,56 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Prakruthi Jayant</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -3588,26 +3588,26 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Priyanshi Patel</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -3618,86 +3618,86 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Excused</t>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -3708,26 +3708,26 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -3738,22 +3738,22 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -3768,26 +3768,26 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -3798,26 +3798,26 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Samwel Gitundu</t>
+          <t>Priyanka Umesh Patil</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -3828,7 +3828,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3847,18 +3847,18 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3881,14 +3881,14 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3907,7 +3907,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -3918,7 +3918,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3937,7 +3937,7 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -3948,7 +3948,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3971,14 +3971,14 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -4008,7 +4008,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Srinidhi Rajaraman</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -4027,7 +4027,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -4038,22 +4038,22 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Priyanshi Patel</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -4068,22 +4068,22 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -4091,29 +4091,29 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -4121,33 +4121,33 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
@@ -4158,26 +4158,26 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -4188,26 +4188,26 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -4218,26 +4218,26 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Srishti Michael</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
@@ -4248,26 +4248,26 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -4278,26 +4278,26 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Samwel Gitundu</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -4308,22 +4308,22 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -4338,22 +4338,22 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -4361,33 +4361,33 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -4398,26 +4398,26 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 4 (9/25)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/25</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Payer: History, Overview, ACA and Services</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -4428,26 +4428,26 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Varsha Murli Chhabria</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Week 7 (10/16)</t>
+          <t>Week 5 (10/2)</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>10/16</t>
+          <t>10/2</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+          <t>Payer: Medicare and Medicaid</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -4458,26 +4458,26 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Wesley Tey</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Week 1 (9/4)</t>
+          <t>Week 6 (10/9)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>9/4</t>
+          <t>10/9</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>U.S. Healthcare Ecosystem Overview and History</t>
+          <t>Provider: History, Types and Challenges</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
@@ -4488,26 +4488,26 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Wesley Tey</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Week 2 (9/11)</t>
+          <t>Week 7 (10/16)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>10/16</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -4518,26 +4518,26 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Wesley Tey</t>
+          <t>Srinidhi Rajaraman</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Week 3 (9/18)</t>
+          <t>Week 8 (10/23)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>9/18</t>
+          <t>10/23</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -4548,26 +4548,26 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Wesley Tey</t>
+          <t>Srishti Michael</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Week 4 (9/25)</t>
+          <t>Week 1 (9/4)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>9/25</t>
+          <t>9/4</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Payer: History, Overview, ACA and Services</t>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -4578,22 +4578,22 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Wesley Tey</t>
+          <t>Srishti Michael</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Week 5 (10/2)</t>
+          <t>Week 2 (9/11)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>10/2</t>
+          <t>9/11</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Payer: Medicare and Medicaid</t>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -4608,26 +4608,26 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Wesley Tey</t>
+          <t>Srishti Michael</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Week 6 (10/9)</t>
+          <t>Week 3 (9/18)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10/9</t>
+          <t>9/18</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Provider: History, Types and Challenges</t>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -4638,28 +4638,628 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
+          <t>Srishti Michael</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Week 4 (9/25)</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>9/25</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Payer: History, Overview, ACA and Services</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Srishti Michael</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Week 5 (10/2)</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>10/2</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Payer: Medicare and Medicaid</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Srishti Michael</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Week 6 (10/9)</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>10/9</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Provider: History, Types and Challenges</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Srishti Michael</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Week 7 (10/16)</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Srishti Michael</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Week 8 (10/23)</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>10/23</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>0</v>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Week 1 (9/4)</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>9/4</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>2</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Week 2 (9/11)</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>9/11</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Week 3 (9/18)</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>9/18</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>1</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Week 4 (9/25)</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>9/25</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Payer: History, Overview, ACA and Services</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>0</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Week 5 (10/2)</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>10/2</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Payer: Medicare and Medicaid</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>3</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Week 6 (10/9)</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>10/9</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Provider: History, Types and Challenges</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>0</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Week 7 (10/16)</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>10/16</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>2</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Varsha Murli Chhabria</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Week 8 (10/23)</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>10/23</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
           <t>Wesley Tey</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Week 1 (9/4)</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>9/4</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>U.S. Healthcare Ecosystem Overview and History</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>2</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Week 2 (9/11)</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>9/11</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Patient: Experience, Responsibility, and Paying for Healthcare</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>1</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Week 3 (9/18)</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>9/18</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Patient: Care Delivery – Where, Why, Impact and Challenges</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>1</v>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Week 4 (9/25)</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>9/25</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Payer: History, Overview, ACA and Services</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>0</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Week 5 (10/2)</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>10/2</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Payer: Medicare and Medicaid</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Week 6 (10/9)</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>10/9</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Provider: History, Types and Challenges</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>4</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
         <is>
           <t>Week 7 (10/16)</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr">
+      <c r="C160" t="inlineStr">
         <is>
           <t>10/16</t>
         </is>
       </c>
-      <c r="D141" t="inlineStr">
+      <c r="D160" t="inlineStr">
         <is>
           <t>Provider: Compensation, Education, Burn-out and Satisfaction</t>
         </is>
       </c>
-      <c r="E141" t="n">
+      <c r="E160" t="n">
         <v>2</v>
       </c>
-      <c r="F141" t="inlineStr">
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Wesley Tey</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Week 8 (10/23)</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>10/23</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Government: Policies and regulations, Social Determinants of Health</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>2</v>
+      </c>
+      <c r="F161" t="inlineStr">
         <is>
           <t>Present</t>
         </is>

</xml_diff>

<commit_message>
fix(data): correct Week 12 date to 11/20 and remove incorrect 12/20 label
</commit_message>
<xml_diff>
--- a/American_Healthcare_Class_Cleaned.xlsx
+++ b/American_Healthcare_Class_Cleaned.xlsx
@@ -563,12 +563,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -923,12 +923,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1283,12 +1283,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1643,12 +1643,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2003,12 +2003,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2363,12 +2363,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2723,12 +2723,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3083,12 +3083,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3443,12 +3443,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3803,12 +3803,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -4163,12 +4163,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4523,12 +4523,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4883,12 +4883,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -5243,12 +5243,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -5603,12 +5603,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5963,12 +5963,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -6323,12 +6323,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -6683,12 +6683,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -7043,12 +7043,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -7403,12 +7403,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Week 12 (12/20)</t>
+          <t>Week 12 (11/20)</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>12/20</t>
+          <t>11/20</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">

</xml_diff>

<commit_message>
fix(data): change all Anika Rahman Maria absences to Excused
</commit_message>
<xml_diff>
--- a/American_Healthcare_Class_Cleaned.xlsx
+++ b/American_Healthcare_Class_Cleaned.xlsx
@@ -1211,7 +1211,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Excused</t>
         </is>
       </c>
     </row>

</xml_diff>